<commit_message>
just creat the new LUR input
</commit_message>
<xml_diff>
--- a/revised input 10252018/HOA COA input_20181024.xlsx
+++ b/revised input 10252018/HOA COA input_20181024.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qingye1009/Library/Containers/com.microsoft.Excel/Data/Desktop/matlab_Ye_2018a/new20181023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Box Sync/from_dropbox/ACE hugh/ACE R/ACE_LUR/local_lur/revised input 10252018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0893AF21-2485-5F42-9B4F-CEADE1888C6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B0DBB1-E7FE-8546-9D99-B69617CDA2C7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9880" yWindow="460" windowWidth="20780" windowHeight="15720" activeTab="1" xr2:uid="{6C74B704-F184-F64F-B957-A9CD66CB0618}"/>
+    <workbookView xWindow="4820" yWindow="440" windowWidth="20780" windowHeight="15060" xr2:uid="{6C74B704-F184-F64F-B957-A9CD66CB0618}"/>
   </bookViews>
   <sheets>
     <sheet name="200m" sheetId="1" r:id="rId1"/>
     <sheet name="polygon" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>200cell id</t>
   </si>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8876722B-0555-6746-B7BE-66EEB47079E0}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55338549-D445-C545-8598-799B8FA11A47}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,6 +1245,124 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>281.34965257990831</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>1532.2180587484145</v>
+      </c>
+      <c r="E17">
+        <v>86.260057972653698</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>2661.7386417754592</v>
+      </c>
+      <c r="E18">
+        <v>3441.956135321805</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>3074.0429501731896</v>
+      </c>
+      <c r="E19">
+        <v>1134.9005388599323</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>3718.1400000000003</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>2215.473213027663</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3020.0883074217782</v>
+      </c>
+      <c r="E22">
+        <v>1437.5051889711117</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>1870.5922728956496</v>
+      </c>
+      <c r="E23">
+        <v>522.13342638172537</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>2507.8337900525871</v>
+      </c>
+      <c r="E24">
+        <v>1798.7888624100087</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>1269.8810578609045</v>
+      </c>
+      <c r="E25">
+        <v>780.06135478955309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>